<commit_message>
generate report to exel file function added
</commit_message>
<xml_diff>
--- a/usedData/accounts.xlsx
+++ b/usedData/accounts.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -412,87 +412,807 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>0xaf7Bc9f7395255dA34b394Da375e540724aFdb70</v>
+        <v>0xeB36C04440371ad32dC9D03b50580a2603711c1B</v>
       </c>
       <c r="B2" t="str">
-        <v>0x08e0c7b75d3faa4e7b389c1810abf74155039b038fc976a351d78ab3c0f016af</v>
+        <v>0x3333a1d4c55b05ca5d10ed252198bba9f012863ca8b96aac8cc832d7b57a52c9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>0x7c11fB3794043eB66CF781AA948F1CE83810bf06</v>
+        <v>0x17eE90e087db3d87Ba6EaF06be9A28446E4Ec0be</v>
       </c>
       <c r="B3" t="str">
-        <v>0xff349e75dfd8f5f9bd3682ec5af5f42083fc179a332217181cf0540a7c10c65c</v>
+        <v>0x8f113d346dad7517fde2e0867c140abac04dfc94fbcfd0b2e853f4f43eb5316f</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>0xcfAdF4D06e4996f3Eb266a0D756696c767f71525</v>
+        <v>0xc56ce77138A5afC8EC830CA9d7491F23bA8DE0b2</v>
       </c>
       <c r="B4" t="str">
-        <v>0x355ce2a3901a9a2127b7d77285959ec7efabf52360829407ec8ab2595ea55c0f</v>
+        <v>0x2b0bca01e14ca0b9c05c3ee2db6e1e9dfadd8bc8f49a6851da309a78f5375313</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>0xdC29ad46683639aB29E0C96AdF4708EafD743917</v>
+        <v>0x40E5c5BE8330f834F1b964D978f27E9625ebe0dB</v>
       </c>
       <c r="B5" t="str">
-        <v>0x7e53b6531e9f037a704af68bcab18826ec4094365c2316e592dc4250f2dd806d</v>
+        <v>0x3ad365ae14fddbfad76bde5a503fe4b709d6f6df9b586da460576e2a6f9737d3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>0x14e87943485c2F9E8ce3371de3162523d1F13513</v>
+        <v>0xd7455869da881e8BED13fb571651Aa22974D0e55</v>
       </c>
       <c r="B6" t="str">
-        <v>0x87dc6b5dca15b51b5db468dc3bf77f4cc5282b24a7e0fe9919e806e82fd732a1</v>
+        <v>0xb0cbcaee46f517990f173e1dcea614aa1295c1639b9a20f29ac13182c9e8fe89</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>0x9b29194CB95F753c507cc462698695AdAB45B72C</v>
+        <v>0x25F998c9AC86CE46822F7DE8F200bEc3e25d3D28</v>
       </c>
       <c r="B7" t="str">
-        <v>0x50d4b15b73715996169abd7cc23c05bcfb9b917d651c23e1b0617b9bf1016412</v>
+        <v>0xea4c1ed729900d3d7b866dd7bd13eebdf82f5078fbbd88118794b6630a31cc4c</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>0x9Ea04CEC17409684d8D631EfA238659c6B17023F</v>
+        <v>0xF53F497953d620c0b1182D11272DF5a735Cb96F3</v>
       </c>
       <c r="B8" t="str">
-        <v>0x3898cfbac72a65eed8b0000e4c5383352998dbdb7ea68501e4f2f357220710dd</v>
+        <v>0x4e35752821846e050548ed4903db7bb2a63ae4cfb2a9157421b5660fc85e23c7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>0x0Dd6D78F5f5553a1bb5D3CC53385B6eF35996460</v>
+        <v>0xBe2cd78E9282669f30b184836b13e112d0DC28f3</v>
       </c>
       <c r="B9" t="str">
-        <v>0x2f3eb657548b2e29f93b85392fc003c8a11b145af29b078afce21815dbe0468e</v>
+        <v>0x4986e2dc1cf61ee01692b90223d2a179e5df69b49752b5c21df4bcf792328d64</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>0x87Eb1782139812ccfd900776D573899479f1992D</v>
+        <v>0x8fF5D7EE2AE84c649A88E467786158b6ced2ccdF</v>
       </c>
       <c r="B10" t="str">
-        <v>0x325d08f2bde380b1b353b7947b9baaa6ceb833f595fd4f9a76ea67e0d6c8891a</v>
+        <v>0xb8adc221bae9c0a91e7e12013aea87949a305c9f369632c19ff41832748dff12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>0xBeC1b78399c74C3B8ca13a41a9B43580f801178C</v>
+        <v>0x0aE58B4CF549E02158B90B5A4f2266B43B93423B</v>
       </c>
       <c r="B11" t="str">
-        <v>0x16b3b854931a74f2604a343a26560a22e77d9f943954c3080c9a8e47ab382406</v>
+        <v>0x6e1d641a124edf0f84952e1593d5044984461cd4d46ab2c142b951765cd0786e</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>0xF88a258cCF9739D9a6756808B2369BD27d65F425</v>
+      </c>
+      <c r="B12" t="str">
+        <v>0x33fe4b9a2b71b1bca10215c84387f767aa764599b8474b5505577d58d390ac54</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>0xE3ad35525F481d4ECcBdF7829e96B3b5CFa4e894</v>
+      </c>
+      <c r="B13" t="str">
+        <v>0x410706279ace3adf3ec4f40a2f3734f6cd988c89fc616f20f1ae04aa49076911</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>0x169E533AE1291a49e4364B1Fc7eCfEF5aEe49F29</v>
+      </c>
+      <c r="B14" t="str">
+        <v>0xc42dc21c7e5903a11c9ae9817d9a58e65dd740cc9c671edfad2d2ef17ea32b37</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>0x95329141d442c6622cA34ba877d63f05E5687A2A</v>
+      </c>
+      <c r="B15" t="str">
+        <v>0x193db2e7803d0bb8cda7a9b6ab1a0ae000eefcc4c1c75377c98400d27f91f24c</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>0xc1650F5a520C8C9FaC98Ab2993fd12c1AB5d6014</v>
+      </c>
+      <c r="B16" t="str">
+        <v>0xcfa5f1ae6cc707c5af263a084ea09e2f6013d7838fd14d468ed06a9c8bb5a7d1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>0xDBF615775287c0D2b63f40f5CF46213b50666C21</v>
+      </c>
+      <c r="B17" t="str">
+        <v>0xb5912a92d885b5485f0ab01e964a86ce05d5f21a2d818e54a6ec374f6b1f8c6e</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>0x3304540fb7613c913Bf7fD7aa0b7f74A115160C1</v>
+      </c>
+      <c r="B18" t="str">
+        <v>0x85f0876d48e659660d2fa636f6ba5d01b1a524774416e258ded154e4f8929b9e</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>0x995e5D7693D55f719492bba5eEda52fd5BFe4623</v>
+      </c>
+      <c r="B19" t="str">
+        <v>0x94b18db127735636c26a5c2a52d92d30bf7917b2c7170c4c9517796f6f17964c</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>0x09068aB77BCaD3b08AFF04AA7d9c0395aFB1daC9</v>
+      </c>
+      <c r="B20" t="str">
+        <v>0xf1b7182565880b943712008f1f01bd56444851955b82e6f56f463e2cdbe18313</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>0x101242523809CbA8E6C89753a60aF4745FeB2863</v>
+      </c>
+      <c r="B21" t="str">
+        <v>0xffa1ef768d971c95eda6dd71253996fa6fd584e207e803bd1fb3eed235bba210</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>0x4a686e2C427ef785ce1C0f750CB28d459f677356</v>
+      </c>
+      <c r="B22" t="str">
+        <v>0x3a332ceee2e8ba3d478ed9495b7c1533d49396d8c51f38ea8291f03077117f17</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>0xC48CdF7D59ea4660d66543a5B91Beb6Da59cf315</v>
+      </c>
+      <c r="B23" t="str">
+        <v>0xc83518b548e9aeb20a962b03ca741f0c5dba8647ae4aa5730fa66cfb70046a4d</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>0x0043911dA2284cEcD5dc6520BD9770e734456a5d</v>
+      </c>
+      <c r="B24" t="str">
+        <v>0xdf499a775db303844bc09dcbddf0bcaed3015ef59ed6b362ac85d1fb34b52f81</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>0x66014db8a447D0f32F35CbB60e3444bcb82D7872</v>
+      </c>
+      <c r="B25" t="str">
+        <v>0x2d9ba4ca1d2bfa725dacfff0d1865650d9c7a0dd2d67884225cbfb266e2202cd</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>0x061e33ca1863c163A58638cF992dea82F517Ca9a</v>
+      </c>
+      <c r="B26" t="str">
+        <v>0x122debdc04aa8c4d72a32e62dfcbcf48854a763af669935488ae28933509f60a</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>0xA8AF3ee5ec64Ce30f3249CdfbaE95f607F76415E</v>
+      </c>
+      <c r="B27" t="str">
+        <v>0x4fa7eaf80bcfcbf65cbb1b50d7ad550f5049aa6f5e3cef20c1aaabaff96e7b5c</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>0x77C7bfC82a0D6899aE48761c32AA85E49F8dEc4d</v>
+      </c>
+      <c r="B28" t="str">
+        <v>0xf2ee0b5fa03fd2f544166ca07fdc6cc79bdeb0e95ede723a1ec7c41397dfa7b3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>0x56b4903c02cE7e475dFF72F51749F21599831391</v>
+      </c>
+      <c r="B29" t="str">
+        <v>0xc196798c1d56e99241019b6fa82d39b5f6a548a115ed37038fd97f3a3843600b</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>0x4C227642E1c1B49CDE2fa9b455b1437737daD142</v>
+      </c>
+      <c r="B30" t="str">
+        <v>0x03cfb21d3deb520f1d8f2dfa8e6698f154c82b29fd831230d4559b0ebb7b5dee</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>0xB76bF1cC4e1fC6AeDDd5d236AC84D6CdD43DFCA2</v>
+      </c>
+      <c r="B31" t="str">
+        <v>0x8a2cc481c4c2603dacc097aa89630014484704e6d6d7ce0ca4387bf3344d6f32</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>0xDF7FE31aaF34ABe2eF239b8Aa302Adc080a99210</v>
+      </c>
+      <c r="B32" t="str">
+        <v>0x17cabd0167a617b2222cde0b4667a343fdc4b7b1b25cf96a720683fa6775695c</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>0x2a9C346a2c4D28eF8e046E602530127F4993a473</v>
+      </c>
+      <c r="B33" t="str">
+        <v>0x12851bad09d722a62b4b6f3680b4e84618829b4b6ac8015112532352779d9ac3</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>0x4D3dF0aFcC4eF60b18f76F3F49AD2eda81584341</v>
+      </c>
+      <c r="B34" t="str">
+        <v>0x41ba2d27357708f9644569fd9b6dd3bf5aac6d0bd587c57dc7297899fb3090ab</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>0x0bAE61ED98E74b9f0dA8a98eeB483C9faD648457</v>
+      </c>
+      <c r="B35" t="str">
+        <v>0x06545c395a92dbf10987772278ee130d143a0296431cc3d067d8b65fb0601104</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>0xb0010FDf179Dce065901823926E34D16AfB6E280</v>
+      </c>
+      <c r="B36" t="str">
+        <v>0x20eaf1b52a01bcc81563092c31a161e7b26d62ab24917ebcc5287ec689f77c0e</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>0x4011E7e2D22128549B0C90C66C52AB9c7FB1769A</v>
+      </c>
+      <c r="B37" t="str">
+        <v>0xf145a6ccac673a9e8a9d502b215f10b51b4e77499a53d1c28b31de4ce0b8f4b5</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>0x368fCe22B4488c379dDFF56bA8956a78B34fBC10</v>
+      </c>
+      <c r="B38" t="str">
+        <v>0x40ee2872cd029c3febc8da4fedc06794a78f0d8f135c213787fd7e9ea73111c0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>0xD86158f53F7b598323C68b8445fD3e0A09CEB673</v>
+      </c>
+      <c r="B39" t="str">
+        <v>0x932edbfcb3db5c35d251d7ea851d08ffb4ae2f359f3be788190135f690fa24d1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>0xD4E8274Ab1Bc22880F7eb4b95f3964BfCb54723e</v>
+      </c>
+      <c r="B40" t="str">
+        <v>0xe8ff99cad5958a6fc8813d6b335b638a8a41dcf8b8ea8821eb2bca1b0ca06d47</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>0xa28ffCC852CB793322BdA293D66eF79aee26811B</v>
+      </c>
+      <c r="B41" t="str">
+        <v>0x51ce38a3973e25a20a7658aab80a3834493abed9799cc48cad409cbc63131817</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>0xbd866e30F8fD875B5b087a9A24F8F99b911217C0</v>
+      </c>
+      <c r="B42" t="str">
+        <v>0xab24edf094e3d3fc987a2b43e45d20f2c3b5ece047b2ec9c7652d5f81a9d238b</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>0xcaa2aabd5C1b5b032C5A262a2025d6c88192eD8C</v>
+      </c>
+      <c r="B43" t="str">
+        <v>0x3c9394967cd0994c868471e25892a2b744fd599968325d6a5c3a3b49acd23224</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>0x9eCDA2a8fEaB96ea57442F420358FDCa8500f1CC</v>
+      </c>
+      <c r="B44" t="str">
+        <v>0x49fb069e32594dcb559e9cce13922d3d11a4e74c86ba558c823038271088351f</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>0x8510a3f7af6c517B3D46ff649163045B9f8f88F5</v>
+      </c>
+      <c r="B45" t="str">
+        <v>0x39a41f0cafa6148b97c075ff641035263855f4fceabd04e5a74e99d47c63b9d4</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>0x4E086b25F327fBd810D32E410Da6ab3750fA5c3E</v>
+      </c>
+      <c r="B46" t="str">
+        <v>0xe47ddd5b7cfa8426fbb1dc33cbc043666138cd5d13b7c862521585b5dc59182c</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>0xB32e22b5E09e24B552b33f723458ADE7B416319d</v>
+      </c>
+      <c r="B47" t="str">
+        <v>0x6e62526ce4919cb68b7658c7fe21c740cea970c4b9c3cfc0c2d4155c21f3dbdc</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>0xAfc9653D38D34AF30fe9736F97Ce12BbdaafcbC8</v>
+      </c>
+      <c r="B48" t="str">
+        <v>0xe32ce93f861cf20d4d425777a6a9ef7e075d35a16d2e44ce4ee1f1d7d37ea541</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>0x8335033Ac9BF5aaD116904434293dB148af04Ba0</v>
+      </c>
+      <c r="B49" t="str">
+        <v>0x8084ee6e7ce255b1bf634a05d1fb9149a13d96d1ade4ffe72b41c29cd996eab4</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>0xCB81Bd705FfE5D91aCB98D64c4667A348732b0c2</v>
+      </c>
+      <c r="B50" t="str">
+        <v>0x640062007842aa23d4f8f1965e920781b61779de7ce13afe95863618166145dd</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>0xA38F1490e9f55DdB6C308B67B597bf995CDF2E77</v>
+      </c>
+      <c r="B51" t="str">
+        <v>0x899523db4f8747cca40765812723001c15812735771f918f71919da4364beaa7</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>0x6B4FBEE05A1CF0B6d74Fa683B6B039c72699058E</v>
+      </c>
+      <c r="B52" t="str">
+        <v>0x4222126c5a1b370613982d5b4e05fa20245b91c8706f50e5cb173f0fa895b14c</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>0x546E1BfB8E9B193C8970f9A2f82e15473e0c52b2</v>
+      </c>
+      <c r="B53" t="str">
+        <v>0x96e5b4f087baeeab96cdc84740a2e145cfe87a712ebb29bba533f9e82fb1bc89</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>0x22f03ae99488E801aaF797BECECFDA390571884D</v>
+      </c>
+      <c r="B54" t="str">
+        <v>0xf42e635156139f76c569902244ab0977cc76e96fc1c4faaa125ad29b6ed8a992</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>0x14b6bA81bB72eb635f655b4baAFC09350daAb188</v>
+      </c>
+      <c r="B55" t="str">
+        <v>0x6f65906f87568a8343eb50b36121bc692729f94caa382cddc7c3028df3e11f20</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>0x5388f6482e1b2595ae6435DA5AF130793770bBe3</v>
+      </c>
+      <c r="B56" t="str">
+        <v>0xc31b67fb1f1bcbbaea3ce76635ba7e121518dccc7e67591f08a6928f96f5083e</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>0x4B72FD457bc5B115ff3CE209004Be1e8C0105c6f</v>
+      </c>
+      <c r="B57" t="str">
+        <v>0x15d2aaf2af1ef4e10d3318a9ba3008a2e1ccd6eb0141f7a3e33c9eb767df5947</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>0x2490d763C14dB6bF4aAeF03fDc8AacC241c67Ef1</v>
+      </c>
+      <c r="B58" t="str">
+        <v>0xbffdd9eb0159e4e748d2689fb336f8be2e0eb05ed543d246bb4359739496b33b</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>0xc13cF0B71f8478BaC66120359a0295fb7553Cd8a</v>
+      </c>
+      <c r="B59" t="str">
+        <v>0x729e1f7c2f1ea53c61cebcface690d88fc8c4858490ff84c8db7ef1419bf8787</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>0x871E6F501BA38d78458f6fb17dd1984eACbE7A00</v>
+      </c>
+      <c r="B60" t="str">
+        <v>0x24c6ee551e2827b13dec61f78a3d01903b635878700e0ea0e30a81fd3ea4719d</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>0x0bf58a640a4365c0423C53c33481a1c5fc1Fe12E</v>
+      </c>
+      <c r="B61" t="str">
+        <v>0x6108ded0be27c7fb0cff4770b498e585fd23e8a2e3707c6515fc2e0599f99e20</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>0xcb2246A7eb5C07465BB3e25CA84c20FC68AB4Fbc</v>
+      </c>
+      <c r="B62" t="str">
+        <v>0xc2b2b8a27cb9cde73f966b3e9c1c06a1718bf8682b241a9ada330a7602837845</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>0x55582D6838f2f8E7b4F0190989564ACc4ce193b3</v>
+      </c>
+      <c r="B63" t="str">
+        <v>0x018ff362d550495ceab57c0345abeae5066c0842f07b832967f216ab0329b4d7</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>0xa013Bbd83E80C6a74a5711e59BEc90be9A1bd615</v>
+      </c>
+      <c r="B64" t="str">
+        <v>0xd6cc5d4a11487855731dac295de03eb0cee7086f234fe83d31d4f546c936155b</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>0x1028E785275909312B3145636E5a3595a6C6314D</v>
+      </c>
+      <c r="B65" t="str">
+        <v>0x059c74fe9d2993a57f33813e5d03d716a68cc12bc347dcd6ca7c87c0e703cb16</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>0x081E82d0067F7a465d57A747Be68F85A4D5821fb</v>
+      </c>
+      <c r="B66" t="str">
+        <v>0x9f07d2cd8104fcb3a3a0754d6a1ffe5ce04e4fef2340740dea9f7b7004f2f729</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>0xfCf188335f12a4b89dd741A59355A2724CEdB305</v>
+      </c>
+      <c r="B67" t="str">
+        <v>0x7eefcd3148dc976471edd0512add3c0a092fd88b429965f40d3e3e803c83aec9</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>0xDcd7b7e871231cc732f6d4E261d6136637Abe067</v>
+      </c>
+      <c r="B68" t="str">
+        <v>0x7ca8dd7bffc36da21e24a816714311da9fd4b8d1f24624d675fc8f3f7ac20b11</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>0xBda69672852FE9Aa7FA785C94Dcee15828D1073B</v>
+      </c>
+      <c r="B69" t="str">
+        <v>0x776f3aeab4c9dd962c1c6a87f3559a9e5207e4d6a156e434f2eda944e3fe6817</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>0x0e0B0787E3BcaB9bD6a7f85576F912d91ED45d83</v>
+      </c>
+      <c r="B70" t="str">
+        <v>0x579bd938f0ca02d99c8d29848c61652a015078d344239ad2221393775f53ba79</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>0x86079b7c0126d4b7eEceBa8deEa86b1B1edDEF68</v>
+      </c>
+      <c r="B71" t="str">
+        <v>0x0e74ec572350a161afa5fa14c785724c581593795244285669fe8c22814789c1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>0x4C21d410F370d09AE2B8E6A0f0502B08517193f2</v>
+      </c>
+      <c r="B72" t="str">
+        <v>0x881596697a8a02b2fec84b6aa354c77f02b49c833a648a645ba896be337e2b0d</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>0x0C94aF6ec23d7D60A5D8Ed7cdA9C913332885CE2</v>
+      </c>
+      <c r="B73" t="str">
+        <v>0x7918a63b5c79551f8681a615ebc5c60a3519dff405c7f867e6eb649eb6a1074a</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>0x74dEa92dF340Bc2486469237ADCe919dA5DBF4B5</v>
+      </c>
+      <c r="B74" t="str">
+        <v>0xa2700ccfd3e512b659f678d7e4da6272f8e93e0cd0e15b592ece9afabcba5919</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>0x500a9366087271399cd595675e64197faa0A06A3</v>
+      </c>
+      <c r="B75" t="str">
+        <v>0xfcd6cf6158f0ec121095ec07e57b73777eee0703b1d456a5effd956ad768bbcf</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>0x7B66590C20B175836e6a0CeE0D982cb4349bD627</v>
+      </c>
+      <c r="B76" t="str">
+        <v>0xfbf577559e0f9d1d09535d17ab03969dd0fc095d2f4f873bac51a354cf1e4516</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>0x7e0e25c2720234E990a2bEF23ffe6400694d6ec6</v>
+      </c>
+      <c r="B77" t="str">
+        <v>0x196e8248e8b37c5456b1168941b1e216a3f17a3920bc4879215598b82047e24a</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>0xbC0b8650819dfb9923Cb81b6F3d1C40c1DE5e3aE</v>
+      </c>
+      <c r="B78" t="str">
+        <v>0xa6bdc698cabd6c24db8744fa99d1f772f993ad8ccf23e8fac99db57b3b9c114f</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>0xd2C7d629cf21CB21F007b08B17552aC966Ec301B</v>
+      </c>
+      <c r="B79" t="str">
+        <v>0xc42a46ea53ddf31d14ad0abd47ed7dd77ffcf0233e10e6bdf78f2aacefe2b94b</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>0x9Fd5c5AEceBE7061cCB5469a89BAF7F9da8805d4</v>
+      </c>
+      <c r="B80" t="str">
+        <v>0x6af11d36bd54a737d6d19627efdbdb182140c879e8703a264424adb3cdc37bf4</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>0x447A480fa600532D4a6e4ABec8B3D1A74855e9eb</v>
+      </c>
+      <c r="B81" t="str">
+        <v>0x16bd2a7f9400a923ea531f38f5a0ecadedf5eeda4b2bff6c0ba6e34904cb0cf3</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>0x37604EC1812e989F57807795704459A764F8c391</v>
+      </c>
+      <c r="B82" t="str">
+        <v>0x771c7816fbe689fa807ad283fc030d0e5e1cc7cfd575554aa2c28120774f9255</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>0xFab059bF7B3c41b510623740E838A905644e5F38</v>
+      </c>
+      <c r="B83" t="str">
+        <v>0x9b329fd078c05ac77d72aa0cd710b0d17b19dd2ea5e657bfddf8e6fe10bea0e1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>0xdB90a8C901DdC7A8749d2474E75591CC2EF80533</v>
+      </c>
+      <c r="B84" t="str">
+        <v>0xfaaace18da70c9b29a2af6fd1afb305d9d1c28b959d57bdee93b8d2b98d95c77</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>0x38560966B45a84d72d14d2f8f1aF224245b70cb5</v>
+      </c>
+      <c r="B85" t="str">
+        <v>0x74a313f5e37f44f4d86426a3f57a43ef0edcab314aa9d818c121ef4a63837caa</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>0x88De2261d3e6d51BdC86e936F9532E82b530e99A</v>
+      </c>
+      <c r="B86" t="str">
+        <v>0x8a16b62213252fc619ad0adb17e2288e21ee41852d68b0273d9a670d9ba301bf</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>0x55200EA1afAd1c237DFC499771EbB852C15ef1B5</v>
+      </c>
+      <c r="B87" t="str">
+        <v>0x25cff1732245ced2909ac9d6b7633526db8ac4310a2940f02c8ac77da1679934</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>0x7B46F243E7d42E22509f6E1CF27d0bC78F4518A6</v>
+      </c>
+      <c r="B88" t="str">
+        <v>0x15a3d82e1e7e0fc98644264e791b927273487979fbcc83cbc6d056607e6ea3ed</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>0x953b75a4D5Bf4619385b04D63Dcb5B826bce3BbE</v>
+      </c>
+      <c r="B89" t="str">
+        <v>0x3b4efdc64c65b3df2bb3059f27cbc86ede3dd35fbb1c0c6aeb5bc9b80dc06fe0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>0x4773b55Dc7F2273d079C124D3A4dBe52cF298492</v>
+      </c>
+      <c r="B90" t="str">
+        <v>0x88a91db7b61e7938ca7708525c4ce13d34ff94cd9908184b44643d86b28363f7</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>0x1066F6e9a096CAf3892f7413accB7e365cF549C2</v>
+      </c>
+      <c r="B91" t="str">
+        <v>0x1fb66c0477c40fb9737a55aadf8b391c8c85dc558a07a562dcb6acab13c64529</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>0x6734Dd0CCBF17B9ed6241e2Bf9A4816297BfC933</v>
+      </c>
+      <c r="B92" t="str">
+        <v>0xea4ade9357bdd598e2446acb3ef0dd60bc25d22e25df45e7ef94ba61dc93764d</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>0x0aF458D83A0bfeD409a39BdE58E529e6009f80aA</v>
+      </c>
+      <c r="B93" t="str">
+        <v>0xcef77ac0e19fac0b3b641c26dec3d7e400c42afc4cb6cb783535323df90b8a0c</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>0x2F0Dcf923CdB2D1a41DBC7bE9BC9b7d89478d560</v>
+      </c>
+      <c r="B94" t="str">
+        <v>0x5c82616435fb7ab3bae359c4f6b3b2e1c64f4cc854f447fb72684ab2f667df0d</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>0x0Df9db87F174f747b92aF926d6C2E430292739Fc</v>
+      </c>
+      <c r="B95" t="str">
+        <v>0x152d5db3a46ce9fbcde89e2683c058fed622b92606cfc74d03b67a386835f07d</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>0x9197779C8B39ea3730993B9845c8D739FC282e9e</v>
+      </c>
+      <c r="B96" t="str">
+        <v>0xeb0080aceb698188465cc1a9e2d20e46b921ee4171c3ec2543a2a1fe7a65c6ed</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>0x61a074D16b339F4CF9acbeC09B5E38538AA5E078</v>
+      </c>
+      <c r="B97" t="str">
+        <v>0x7b93a02d5c518293ca5b7625a4d8f56c1eebcdb910cf42823a4bf5c1961600c0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>0xdacb0Fd4765E29eD7b057394Bc7c3D7F2a8987aC</v>
+      </c>
+      <c r="B98" t="str">
+        <v>0x27f0a91221daefb08fd18f744b229b4ce40383a0d6ff2c9658ce1f64b7f4d390</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>0x6D18C744823102C9767018582CF275A2CFf9aB2E</v>
+      </c>
+      <c r="B99" t="str">
+        <v>0x8e153c784e0e8579dcd54ce091c3cd06f0d5f893f6729ee8da7ac8b702789940</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>0x69bAD9Db2fD21A3A429EfAE99393318C7b2bA815</v>
+      </c>
+      <c r="B100" t="str">
+        <v>0x13f96ba06e6b66c4817892505e0286f02eb16ae6c082ad9b96e1ff5406629fd0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>0xab17fEa5A7e77ca83C7d3985B1909e7F6FbD1C5d</v>
+      </c>
+      <c r="B101" t="str">
+        <v>0x5d0f8b48a4e6123a34e235fd20656b77fe9377443d25e08c994af5728087763b</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B101"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>